<commit_message>
updated code & added logs
</commit_message>
<xml_diff>
--- a/parse_jupyter/traffic_columns_in_common.xlsx
+++ b/parse_jupyter/traffic_columns_in_common.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\R011846\Documents\GitHub\mimecast_log_collector\parse_jupyter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49177A3-9365-4B96-B959-6F40CF0D2D4E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72CD3B2-1083-4E81-A469-B4AD8934EC19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="57600" windowHeight="26595" xr2:uid="{8B76475E-4961-4DF0-80FB-6ADD7EB48B6E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="57600" windowHeight="26592" xr2:uid="{8B76475E-4961-4DF0-80FB-6ADD7EB48B6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -300,7 +300,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,6 +342,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -376,7 +395,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -415,6 +434,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -733,19 +764,19 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="17.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="88.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="3" width="17.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="88.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5546875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>34</v>
       </c>
@@ -765,7 +796,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -782,7 +813,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -796,7 +827,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
@@ -808,19 +839,19 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="10" t="s">
@@ -833,7 +864,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="10" t="s">
         <v>11</v>
@@ -843,7 +874,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7" t="s">
         <v>4</v>
@@ -855,7 +886,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -870,31 +901,31 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="17" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="15" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="12" t="s">
         <v>17</v>
@@ -904,7 +935,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>8</v>
       </c>
@@ -916,7 +947,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>28</v>
       </c>
@@ -928,7 +959,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>15</v>
       </c>
@@ -938,7 +969,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>6</v>
       </c>
@@ -950,7 +981,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
       <c r="C17" s="12" t="s">
@@ -960,7 +991,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>10</v>
       </c>
@@ -974,19 +1005,19 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7" t="s">
+      <c r="B19" s="14"/>
+      <c r="C19" s="14" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="12" t="s">
         <v>13</v>
@@ -996,7 +1027,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12" t="s">
@@ -1006,43 +1037,43 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="7"/>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="14" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B23" s="7"/>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="14" t="s">
         <v>25</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B24" s="7"/>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12" t="s">
@@ -1052,19 +1083,19 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B26" s="7"/>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
@@ -1074,8 +1105,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="12" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B28" s="12"/>
@@ -1084,8 +1115,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="12" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
         <v>3</v>
       </c>
       <c r="B29" s="12"/>
@@ -1094,8 +1125,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="12" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B30" s="12"/>
@@ -1104,42 +1135,42 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B31" s="7"/>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B32" s="7"/>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="14" t="s">
         <v>21</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="12"/>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="12" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="12"/>

</xml_diff>